<commit_message>
Change to end_bias to be 3 prime end bias
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/filled/10x_v2/pbmc8k.xlsx
+++ b/examples/spreadsheets/v5/filled/10x_v2/pbmc8k.xlsx
@@ -613,7 +613,7 @@
     <t>Ficoll gradient</t>
   </si>
   <si>
-    <t>three3 prime end bias_prime_end</t>
+    <t>3 prime end bias</t>
   </si>
 </sst>
 </file>
@@ -43644,7 +43644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>